<commit_message>
added evn config to server
</commit_message>
<xml_diff>
--- a/Photo Album App - Step by Step.xlsx
+++ b/Photo Album App - Step by Step.xlsx
@@ -4,14 +4,20 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Sheet2" sheetId="2" r:id="rId5"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName hidden="1" localSheetId="1" name="Z_786CCFAF_7670_4FBA_AB89_96C9221F55DB_.wvu.FilterData">Sheet2!$B$1:$B$1000</definedName>
+  </definedNames>
   <calcPr/>
+  <customWorkbookViews>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{786CCFAF-7670-4FBA-AB89-96C9221F55DB}" name="Filter 1"/>
+  </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="114">
   <si>
     <t>Server - :4400</t>
   </si>
@@ -247,13 +253,13 @@
     <t>GET</t>
   </si>
   <si>
-    <t>GET data -&gt; Select * from tbl</t>
+    <t>GET data -&gt; Select * from tbl (optionally GET can take a URL param to the server)</t>
   </si>
   <si>
     <t>Update</t>
   </si>
   <si>
-    <t>PATCH/PUT</t>
+    <t>PUT</t>
   </si>
   <si>
     <t>UPDATE tbl WHERE id=:id</t>
@@ -361,6 +367,81 @@
   <si>
     <t>If true, then redirect to another page. IF failed, then display a message to the user</t>
   </si>
+  <si>
+    <t xml:space="preserve">If user registration successful, then provide a link to Log in with the same credentials that the user registerd with </t>
+  </si>
+  <si>
+    <t>Update User Profile</t>
+  </si>
+  <si>
+    <t>Display a form pre-filled with my details</t>
+  </si>
+  <si>
+    <t>HTML page with two input boxes - email and password. 
+- Get user details from database based on the userid
+- localstorage would contain the id of the user</t>
+  </si>
+  <si>
+    <t>cookies
+localstorage</t>
+  </si>
+  <si>
+    <t>Send a PUT request to update the modified values</t>
+  </si>
+  <si>
+    <t>1. Create a Stored Procedure and test it. analyze the output from the database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Create an API Endpoint and test it. </t>
+  </si>
+  <si>
+    <t>3. Service at the client side to fire the API</t>
+  </si>
+  <si>
+    <t>4. Pass the data from the front-end to the service and subscribe</t>
+  </si>
+  <si>
+    <t>5. Update front-end accordingly</t>
+  </si>
+  <si>
+    <t>Server set up</t>
+  </si>
+  <si>
+    <t>DB set up</t>
+  </si>
+  <si>
+    <t>Stored Procedures</t>
+  </si>
+  <si>
+    <t>GetPosts()</t>
+  </si>
+  <si>
+    <t>NewPost(newPost)</t>
+  </si>
+  <si>
+    <t>UpdatePost(:id, updatedPost)</t>
+  </si>
+  <si>
+    <t>DeletePost(:id)</t>
+  </si>
+  <si>
+    <t>API Endpoints</t>
+  </si>
+  <si>
+    <t>/posts</t>
+  </si>
+  <si>
+    <t>/posts    { post: "asdfasdf" }</t>
+  </si>
+  <si>
+    <t>UPDATE</t>
+  </si>
+  <si>
+    <t>/posts/ { id: 5, updatePost: "asdfasdf"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/posts/:id </t>
+  </si>
 </sst>
 </file>
 
@@ -420,7 +501,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -448,6 +529,12 @@
     <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -457,6 +544,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -666,6 +757,7 @@
   <cols>
     <col customWidth="1" min="3" max="3" width="26.63"/>
     <col customWidth="1" min="4" max="4" width="70.13"/>
+    <col customWidth="1" min="5" max="5" width="33.75"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2689,7 +2781,9 @@
     <row r="61">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
+      <c r="C61" s="9" t="s">
+        <v>90</v>
+      </c>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
@@ -2775,7 +2869,9 @@
     </row>
     <row r="64">
       <c r="A64" s="1"/>
-      <c r="B64" s="1"/>
+      <c r="B64" s="5" t="s">
+        <v>91</v>
+      </c>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
@@ -2803,11 +2899,19 @@
       <c r="AA64" s="1"/>
     </row>
     <row r="65">
-      <c r="A65" s="1"/>
+      <c r="A65" s="5">
+        <v>1.0</v>
+      </c>
       <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
+      <c r="C65" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>94</v>
+      </c>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
@@ -2835,7 +2939,9 @@
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
+      <c r="D66" s="5" t="s">
+        <v>95</v>
+      </c>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
@@ -2864,7 +2970,9 @@
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
+      <c r="D67" s="5" t="s">
+        <v>96</v>
+      </c>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
@@ -2893,7 +3001,9 @@
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
+      <c r="D68" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
@@ -2922,7 +3032,9 @@
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
+      <c r="D69" s="5" t="s">
+        <v>98</v>
+      </c>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
@@ -2951,7 +3063,9 @@
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
+      <c r="D70" s="5" t="s">
+        <v>99</v>
+      </c>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
@@ -2980,7 +3094,9 @@
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
+      <c r="D71" s="5" t="s">
+        <v>100</v>
+      </c>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
@@ -30391,4 +30507,124 @@
   </hyperlinks>
   <drawing r:id="rId6"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="40.75"/>
+  </cols>
+  <sheetData>
+    <row r="3">
+      <c r="B3" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" s="10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{786CCFAF-7670-4FBA-AB89-96C9221F55DB}" filter="1" showAutoFilter="1">
+      <autoFilter ref="$B$1:$B$1000">
+        <sortState ref="B1:B1000">
+          <sortCondition ref="B1:B1000"/>
+        </sortState>
+      </autoFilter>
+    </customSheetView>
+  </customSheetViews>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>